<commit_message>
The messy 15N db
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
+++ b/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
@@ -651,24 +651,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:S114"/>
+      <selection pane="bottomLeft" activeCell="R45" sqref="A1:R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="7"/>
-    <col min="6" max="6" width="12.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="7"/>
-    <col min="8" max="11" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="11" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="15" width="9.140625" style="9"/>
-    <col min="16" max="16" width="10.140625" style="9" customWidth="1"/>
-    <col min="17" max="19" width="9.140625" style="9"/>
+    <col min="16" max="16" width="10.140625" style="9" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0" style="9" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="9"/>
+    <col min="19" max="19" width="0" style="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1704,7 +1708,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42602</v>
       </c>
@@ -1735,7 +1739,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42602</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>42602</v>
       </c>
@@ -1805,7 +1809,7 @@
       </c>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>42602</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>42602</v>
       </c>
@@ -1887,7 +1891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42602</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42602</v>
       </c>
@@ -1951,7 +1955,7 @@
       </c>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42602</v>
       </c>
@@ -1982,7 +1986,7 @@
       </c>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>42602</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>42602</v>
       </c>
@@ -2040,7 +2044,7 @@
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>42602</v>
       </c>
@@ -2069,7 +2073,7 @@
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42617</v>
       </c>
@@ -2102,7 +2106,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42617</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>42617</v>
       </c>
@@ -2182,7 +2186,7 @@
       </c>
       <c r="S37" s="6"/>
     </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>42617</v>
       </c>
@@ -2223,7 +2227,7 @@
       </c>
       <c r="S38" s="6"/>
     </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>42617</v>
       </c>
@@ -2264,7 +2268,7 @@
       </c>
       <c r="S39" s="6"/>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42617</v>
       </c>
@@ -2298,7 +2302,7 @@
       </c>
       <c r="S40" s="7"/>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42617</v>
       </c>
@@ -2332,7 +2336,7 @@
       </c>
       <c r="S41" s="7"/>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42617</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42617</v>
       </c>
@@ -2401,7 +2405,7 @@
       </c>
       <c r="S43" s="7"/>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42617</v>
       </c>
@@ -2432,7 +2436,7 @@
       </c>
       <c r="S44" s="7"/>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42617</v>
       </c>
@@ -2463,7 +2467,7 @@
       </c>
       <c r="S45" s="7"/>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42671</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>-5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>42671</v>
       </c>
@@ -2516,7 +2520,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>42671</v>
       </c>
@@ -2557,7 +2561,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>42671</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>42671</v>
       </c>
@@ -2639,7 +2643,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>42671</v>
       </c>
@@ -2670,7 +2674,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>42671</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>-5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>42671</v>
       </c>
@@ -2729,7 +2733,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>42671</v>
       </c>
@@ -2754,7 +2758,7 @@
         <v>-0.308</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42671</v>
       </c>
@@ -2773,7 +2777,7 @@
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42671</v>
       </c>
@@ -2792,7 +2796,7 @@
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>42723</v>
       </c>
@@ -2815,7 +2819,7 @@
       <c r="R57" s="7"/>
       <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42723</v>
       </c>
@@ -2838,7 +2842,7 @@
       <c r="R58" s="7"/>
       <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>42723</v>
       </c>
@@ -2877,7 +2881,7 @@
       <c r="R59" s="6"/>
       <c r="S59" s="6"/>
     </row>
-    <row r="60" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>42723</v>
       </c>
@@ -2916,7 +2920,7 @@
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
     </row>
-    <row r="61" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>42723</v>
       </c>
@@ -2955,7 +2959,7 @@
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42723</v>
       </c>
@@ -2981,7 +2985,7 @@
       <c r="R62" s="7"/>
       <c r="S62" s="7"/>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42723</v>
       </c>
@@ -3007,7 +3011,7 @@
       <c r="R63" s="7"/>
       <c r="S63" s="7"/>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42723</v>
       </c>
@@ -3033,7 +3037,7 @@
       <c r="R64" s="7"/>
       <c r="S64" s="7"/>
     </row>
-    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42723</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42723</v>
       </c>
@@ -3085,7 +3089,7 @@
       <c r="R66" s="7"/>
       <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42723</v>
       </c>
@@ -3104,7 +3108,7 @@
       <c r="R67" s="7"/>
       <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42800</v>
       </c>
@@ -3127,7 +3131,7 @@
       <c r="R68" s="7"/>
       <c r="S68" s="7"/>
     </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42800</v>
       </c>
@@ -3150,7 +3154,7 @@
       <c r="R69" s="7"/>
       <c r="S69" s="7"/>
     </row>
-    <row r="70" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>42800</v>
       </c>
@@ -3189,7 +3193,7 @@
       <c r="R70" s="6"/>
       <c r="S70" s="6"/>
     </row>
-    <row r="71" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>42800</v>
       </c>
@@ -3228,7 +3232,7 @@
       <c r="R71" s="6"/>
       <c r="S71" s="6"/>
     </row>
-    <row r="72" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>42800</v>
       </c>
@@ -3267,7 +3271,7 @@
       <c r="R72" s="6"/>
       <c r="S72" s="6"/>
     </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>42800</v>
       </c>
@@ -3293,7 +3297,7 @@
       <c r="R73" s="7"/>
       <c r="S73" s="7"/>
     </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>42800</v>
       </c>
@@ -3319,7 +3323,7 @@
       <c r="R74" s="7"/>
       <c r="S74" s="7"/>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>42800</v>
       </c>
@@ -3345,7 +3349,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="7"/>
     </row>
-    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>42800</v>
       </c>
@@ -3368,7 +3372,7 @@
       <c r="R76" s="7"/>
       <c r="S76" s="7"/>
     </row>
-    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>42800</v>
       </c>
@@ -3387,7 +3391,7 @@
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>42800</v>
       </c>
@@ -3406,7 +3410,7 @@
       <c r="R78" s="7"/>
       <c r="S78" s="7"/>
     </row>
-    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>42671</v>
       </c>
@@ -3429,7 +3433,7 @@
       <c r="R79" s="7"/>
       <c r="S79" s="7"/>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>42671</v>
       </c>
@@ -3448,7 +3452,7 @@
       <c r="R80" s="7"/>
       <c r="S80" s="7"/>
     </row>
-    <row r="81" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>42671</v>
       </c>
@@ -3479,7 +3483,7 @@
       <c r="R81" s="6"/>
       <c r="S81" s="6"/>
     </row>
-    <row r="82" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>42671</v>
       </c>
@@ -3510,7 +3514,7 @@
       <c r="R82" s="6"/>
       <c r="S82" s="6"/>
     </row>
-    <row r="83" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>42671</v>
       </c>
@@ -3541,7 +3545,7 @@
       <c r="R83" s="6"/>
       <c r="S83" s="6"/>
     </row>
-    <row r="84" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>42671</v>
       </c>
@@ -3564,7 +3568,7 @@
       <c r="R84" s="7"/>
       <c r="S84" s="7"/>
     </row>
-    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>42671</v>
       </c>
@@ -3587,7 +3591,7 @@
       <c r="R85" s="7"/>
       <c r="S85" s="7"/>
     </row>
-    <row r="86" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>42671</v>
       </c>
@@ -3610,7 +3614,7 @@
       <c r="R86" s="7"/>
       <c r="S86" s="7"/>
     </row>
-    <row r="87" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>42671</v>
       </c>
@@ -3633,7 +3637,7 @@
       <c r="R87" s="7"/>
       <c r="S87" s="7"/>
     </row>
-    <row r="88" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>42671</v>
       </c>
@@ -3656,7 +3660,7 @@
       <c r="R88" s="7"/>
       <c r="S88" s="7"/>
     </row>
-    <row r="89" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>42671</v>
       </c>
@@ -3679,7 +3683,7 @@
       <c r="R89" s="7"/>
       <c r="S89" s="7"/>
     </row>
-    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>42800</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>42800</v>
       </c>
@@ -3727,7 +3731,7 @@
       <c r="R91" s="7"/>
       <c r="S91" s="7"/>
     </row>
-    <row r="92" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>42807</v>
       </c>
@@ -3768,7 +3772,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>42807</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>42807</v>
       </c>
@@ -3850,7 +3854,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>42807</v>
       </c>
@@ -3876,7 +3880,7 @@
       <c r="R95" s="7"/>
       <c r="S95" s="7"/>
     </row>
-    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>42807</v>
       </c>
@@ -3902,7 +3906,7 @@
       <c r="R96" s="7"/>
       <c r="S96" s="7"/>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>42807</v>
       </c>
@@ -3928,7 +3932,7 @@
       <c r="R97" s="7"/>
       <c r="S97" s="7"/>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>42807</v>
       </c>
@@ -3951,7 +3955,7 @@
       <c r="R98" s="7"/>
       <c r="S98" s="7"/>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>42807</v>
       </c>
@@ -3974,7 +3978,7 @@
       <c r="R99" s="7"/>
       <c r="S99" s="7"/>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>42807</v>
       </c>
@@ -3994,7 +3998,7 @@
       <c r="R100" s="7"/>
       <c r="S100" s="7"/>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>42831</v>
       </c>
@@ -4010,7 +4014,7 @@
       <c r="R101" s="7"/>
       <c r="S101" s="7"/>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>42831</v>
       </c>
@@ -4028,7 +4032,7 @@
       <c r="R102" s="7"/>
       <c r="S102" s="7"/>
     </row>
-    <row r="103" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>42831</v>
       </c>
@@ -4063,7 +4067,7 @@
       <c r="R103" s="6"/>
       <c r="S103" s="6"/>
     </row>
-    <row r="104" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>42831</v>
       </c>
@@ -4098,7 +4102,7 @@
       <c r="R104" s="6"/>
       <c r="S104" s="6"/>
     </row>
-    <row r="105" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>42831</v>
       </c>
@@ -4133,7 +4137,7 @@
       <c r="R105" s="6"/>
       <c r="S105" s="6"/>
     </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>42831</v>
       </c>
@@ -4154,7 +4158,7 @@
       <c r="R106" s="7"/>
       <c r="S106" s="7"/>
     </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>42831</v>
       </c>
@@ -4175,7 +4179,7 @@
       <c r="R107" s="7"/>
       <c r="S107" s="7"/>
     </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>42831</v>
       </c>
@@ -4196,7 +4200,7 @@
       <c r="R108" s="7"/>
       <c r="S108" s="7"/>
     </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>42831</v>
       </c>
@@ -4214,7 +4218,7 @@
       <c r="R109" s="7"/>
       <c r="S109" s="7"/>
     </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>42831</v>
       </c>
@@ -4232,7 +4236,7 @@
       <c r="R110" s="7"/>
       <c r="S110" s="7"/>
     </row>
-    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>42831</v>
       </c>
@@ -4395,14 +4399,7 @@
       <c r="S114" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D114">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="D1:D114"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated version of the db and housekeeping on the repo
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
+++ b/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -198,7 +198,34 @@
     <t>A VEDERE LE DIFFERENZE TRA PRIMA E SECONDA BATCH SI DIREBBE CHE I FILTRI no3 DEL PRIMO GIRO SIANO TUTTI SCOPPIATI. NON SI SPIEGHEREBBE ALTRIMENTI IL BASSO CONTENUTO DI N. GUARDA CHE QUANTITA ALLUCINANTE DI NO3-N NEI SECONDI NONOSTANTE UN VOLUME MINIMO!</t>
   </si>
   <si>
-    <t>NIENTE RF? E CT CS ANDO STANNO???</t>
+    <t>Vol calculations</t>
+  </si>
+  <si>
+    <t>barrel 1</t>
+  </si>
+  <si>
+    <t>barrel 2</t>
+  </si>
+  <si>
+    <t>barrel 3</t>
+  </si>
+  <si>
+    <t>barrel 4</t>
+  </si>
+  <si>
+    <t>NH4 diffusion start on 08/03. Sample collected on 6/03 stayed TA for 2 days</t>
+  </si>
+  <si>
+    <t>missing NH4 lab result from the lab analysis</t>
+  </si>
+  <si>
+    <t>NO RF. Results from 02/09</t>
+  </si>
+  <si>
+    <t>NOTA:(24/05/17): IO HO UN VOLUME ANCHE PER IL TF, CHE VA BENISSIMO, PERCHE' MI SERVIRA' PER CALCOLARE QUANTO N HO RACCOLTO: LA SUPERFICIE INTERCETTATA MI SERVIRA' SOLO PER CALCOLARE UN PARAMETRO PER SCALARIZZARE IL N RACCOLTO AL N TOTALE!!!</t>
+  </si>
+  <si>
+    <t>PER DOMANI 25/05: SPEDIRE I CAMPIONI, MAIL A CEH, POI PREPARARE IL DB "PULITO" SALVATO COME .csv</t>
   </si>
 </sst>
 </file>
@@ -208,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +264,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +320,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -326,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -365,8 +410,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,12 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T119"/>
+  <dimension ref="A1:Y119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4:E9"/>
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,8 +714,8 @@
     <col min="3" max="3" width="9.140625" style="7" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="9.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7" hidden="1" customWidth="1"/>
     <col min="8" max="11" width="9.140625" style="3" customWidth="1"/>
     <col min="12" max="15" width="9.140625" style="9"/>
     <col min="16" max="16" width="10.140625" style="9" customWidth="1"/>
@@ -672,7 +724,7 @@
     <col min="19" max="19" width="9.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,8 +785,11 @@
       <c r="T1" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U1" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>42592</v>
       </c>
@@ -774,8 +829,20 @@
         <v>0.6</v>
       </c>
       <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>42592</v>
       </c>
@@ -816,7 +883,7 @@
       </c>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>42592</v>
       </c>
@@ -827,7 +894,7 @@
       <c r="D4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="33">
         <v>4.0759999999999996</v>
       </c>
       <c r="F4" s="21">
@@ -863,7 +930,7 @@
       </c>
       <c r="S4" s="21"/>
     </row>
-    <row r="5" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>42592</v>
       </c>
@@ -874,8 +941,8 @@
       <c r="D5" s="21">
         <v>1</v>
       </c>
-      <c r="E5" s="30">
-        <v>3</v>
+      <c r="E5" s="33">
+        <v>3.48</v>
       </c>
       <c r="F5" s="21">
         <v>14.87</v>
@@ -887,10 +954,10 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="21">
+      <c r="L5" s="30">
         <v>5.407</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="30">
         <v>16.321999999999999</v>
       </c>
       <c r="N5" s="21">
@@ -910,7 +977,7 @@
       </c>
       <c r="S5" s="21"/>
     </row>
-    <row r="6" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>42592</v>
       </c>
@@ -921,8 +988,8 @@
       <c r="D6" s="21">
         <v>1</v>
       </c>
-      <c r="E6" s="30">
-        <v>3.5</v>
+      <c r="E6" s="33">
+        <v>3.7</v>
       </c>
       <c r="F6" s="21">
         <v>17.41</v>
@@ -934,10 +1001,10 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
-      <c r="L6" s="21">
+      <c r="L6" s="30">
         <v>4.9329999999999998</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="30">
         <v>17.318000000000001</v>
       </c>
       <c r="N6" s="21">
@@ -957,7 +1024,7 @@
       </c>
       <c r="S6" s="21"/>
     </row>
-    <row r="7" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>42592</v>
       </c>
@@ -968,7 +1035,7 @@
       <c r="D7" s="21">
         <v>1</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="34">
         <v>0.95850999999999997</v>
       </c>
       <c r="F7" s="21"/>
@@ -1000,7 +1067,7 @@
       </c>
       <c r="S7" s="21"/>
     </row>
-    <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <v>42592</v>
       </c>
@@ -1011,7 +1078,7 @@
       <c r="D8" s="21">
         <v>1</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="34">
         <v>0.45724999999999999</v>
       </c>
       <c r="F8" s="21"/>
@@ -1043,7 +1110,7 @@
       </c>
       <c r="S8" s="21"/>
     </row>
-    <row r="9" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>42592</v>
       </c>
@@ -1054,7 +1121,7 @@
       <c r="D9" s="21">
         <v>1</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="34">
         <v>0.61875000000000002</v>
       </c>
       <c r="F9" s="21"/>
@@ -1086,7 +1153,7 @@
       </c>
       <c r="S9" s="21"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42592</v>
       </c>
@@ -1142,7 +1209,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42592</v>
       </c>
@@ -1198,7 +1265,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42592</v>
       </c>
@@ -1254,7 +1321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42594</v>
       </c>
@@ -1264,53 +1331,36 @@
       <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>45</v>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="N13" s="7">
+        <v>37.22</v>
+      </c>
+      <c r="O13" s="7">
+        <v>72.11</v>
+      </c>
+      <c r="P13" s="7">
+        <v>17.053684055118111</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>5.8174239423942389</v>
+      </c>
+      <c r="R13" s="7">
+        <v>0.6</v>
       </c>
       <c r="S13" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42594</v>
       </c>
@@ -1320,53 +1370,36 @@
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>45</v>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M14" s="7">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="N14" s="7">
+        <v>64.27</v>
+      </c>
+      <c r="O14" s="7">
+        <v>172.73</v>
+      </c>
+      <c r="P14" s="7">
+        <v>20.170380726635326</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0.2259177150722643</v>
+      </c>
+      <c r="R14" s="7">
+        <v>0.6</v>
       </c>
       <c r="S14" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>42594</v>
       </c>
@@ -1377,7 +1410,7 @@
       <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="30">
         <v>8</v>
       </c>
       <c r="F15" s="6"/>
@@ -1386,10 +1419,10 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="6">
+      <c r="L15" s="30">
         <v>3.8679999999999999</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="30">
         <v>12.097</v>
       </c>
       <c r="N15" s="6">
@@ -1409,7 +1442,7 @@
       </c>
       <c r="S15" s="6"/>
     </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>42594</v>
       </c>
@@ -1420,7 +1453,7 @@
       <c r="D16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="30">
         <v>6</v>
       </c>
       <c r="F16" s="6"/>
@@ -1429,10 +1462,10 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="6">
+      <c r="L16" s="30">
         <v>0.61899999999999999</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="30">
         <v>4.6689999999999996</v>
       </c>
       <c r="N16" s="6">
@@ -1454,7 +1487,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>42594</v>
       </c>
@@ -1465,7 +1498,7 @@
       <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="30">
         <v>8</v>
       </c>
       <c r="F17" s="6"/>
@@ -1474,10 +1507,10 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="6">
+      <c r="L17" s="30">
         <v>0.157</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="30">
         <v>0.13100000000000001</v>
       </c>
       <c r="N17" s="6">
@@ -1499,7 +1532,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42594</v>
       </c>
@@ -1509,13 +1542,13 @@
       <c r="D18" s="7">
         <v>2</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="30">
         <v>7</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="30">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="30">
         <v>0.151</v>
       </c>
       <c r="N18" s="7">
@@ -1537,7 +1570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42594</v>
       </c>
@@ -1547,13 +1580,13 @@
       <c r="D19" s="7">
         <v>2</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="30">
         <v>5</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="30">
         <v>0.17899999999999999</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="30">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N19" s="7">
@@ -1573,7 +1606,7 @@
       </c>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42594</v>
       </c>
@@ -1583,13 +1616,13 @@
       <c r="D20" s="7">
         <v>2</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="30">
         <v>3.75</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="30">
         <v>0.19600000000000001</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="30">
         <v>0</v>
       </c>
       <c r="N20" s="7">
@@ -1609,7 +1642,7 @@
       </c>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42594</v>
       </c>
@@ -1638,7 +1671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42594</v>
       </c>
@@ -1673,7 +1706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42594</v>
       </c>
@@ -1705,7 +1738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42602</v>
       </c>
@@ -1736,7 +1769,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42602</v>
       </c>
@@ -1767,7 +1800,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>42602</v>
       </c>
@@ -1785,10 +1818,12 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="6">
+      <c r="L26" s="30">
         <v>0.36199999999999999</v>
       </c>
-      <c r="M26" s="6"/>
+      <c r="M26" s="30">
+        <v>1.5669999999999999</v>
+      </c>
       <c r="N26" s="6">
         <v>9.82</v>
       </c>
@@ -1806,7 +1841,7 @@
       </c>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>42602</v>
       </c>
@@ -1824,10 +1859,12 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="6">
+      <c r="L27" s="30">
         <v>0.16500000000000001</v>
       </c>
-      <c r="M27" s="6"/>
+      <c r="M27" s="30">
+        <v>3.7789999999999999</v>
+      </c>
       <c r="N27" s="6">
         <v>68.17</v>
       </c>
@@ -1847,7 +1884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>42602</v>
       </c>
@@ -1865,10 +1902,12 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="6">
+      <c r="L28" s="30">
         <v>0.46200000000000002</v>
       </c>
-      <c r="M28" s="6"/>
+      <c r="M28" s="30">
+        <v>2.8119999999999998</v>
+      </c>
       <c r="N28" s="6">
         <v>-3.73</v>
       </c>
@@ -1888,7 +1927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42602</v>
       </c>
@@ -1898,10 +1937,12 @@
       <c r="D29" s="7">
         <v>3</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="30">
         <v>0.23899999999999999</v>
       </c>
-      <c r="M29" s="7"/>
+      <c r="M29" s="30">
+        <v>0.1</v>
+      </c>
       <c r="N29" s="7">
         <v>-0.5</v>
       </c>
@@ -1921,7 +1962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42602</v>
       </c>
@@ -1931,10 +1972,12 @@
       <c r="D30" s="7">
         <v>3</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="30">
         <v>0.19800000000000001</v>
       </c>
-      <c r="M30" s="7"/>
+      <c r="M30" s="30">
+        <v>6.2E-2</v>
+      </c>
       <c r="N30" s="7">
         <v>-9.1199999999999992</v>
       </c>
@@ -1952,7 +1995,7 @@
       </c>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42602</v>
       </c>
@@ -1962,10 +2005,12 @@
       <c r="D31" s="7">
         <v>3</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="30">
         <v>1.129</v>
       </c>
-      <c r="M31" s="7"/>
+      <c r="M31" s="30">
+        <v>0.28399999999999997</v>
+      </c>
       <c r="N31" s="7">
         <v>-2.29</v>
       </c>
@@ -1983,7 +2028,7 @@
       </c>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>42602</v>
       </c>
@@ -2009,10 +2054,10 @@
       <c r="Q32" s="18"/>
       <c r="R32" s="18"/>
       <c r="S32" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>42602</v>
       </c>
@@ -2030,10 +2075,12 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="18">
+      <c r="L33" s="30">
         <v>1E-3</v>
       </c>
-      <c r="M33" s="18"/>
+      <c r="M33" s="30">
+        <v>1.472</v>
+      </c>
       <c r="N33" s="18"/>
       <c r="O33" s="18"/>
       <c r="P33" s="18"/>
@@ -2041,7 +2088,7 @@
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="1:20" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>42602</v>
       </c>
@@ -2059,10 +2106,12 @@
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="18">
+      <c r="L34" s="30">
         <v>0.183</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" s="30">
+        <v>0.36499999999999999</v>
+      </c>
       <c r="N34" s="18"/>
       <c r="O34" s="18"/>
       <c r="P34" s="18"/>
@@ -2070,7 +2119,7 @@
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42617</v>
       </c>
@@ -2080,10 +2129,12 @@
       <c r="D35" s="7">
         <v>4</v>
       </c>
-      <c r="L35" s="7">
+      <c r="L35" s="30">
         <v>4.7E-2</v>
       </c>
-      <c r="M35" s="7"/>
+      <c r="M35" s="30">
+        <v>-1.4999999999999999E-2</v>
+      </c>
       <c r="N35" s="7">
         <v>36.72</v>
       </c>
@@ -2103,7 +2154,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42617</v>
       </c>
@@ -2113,10 +2164,12 @@
       <c r="D36" s="7">
         <v>4</v>
       </c>
-      <c r="L36" s="7">
+      <c r="L36" s="30">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M36" s="7"/>
+      <c r="M36" s="30">
+        <v>-3.2000000000000001E-2</v>
+      </c>
       <c r="N36" s="7">
         <v>50.17</v>
       </c>
@@ -2136,7 +2189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>42617</v>
       </c>
@@ -2162,10 +2215,12 @@
       <c r="K37" s="6">
         <v>7</v>
       </c>
-      <c r="L37" s="6">
+      <c r="L37" s="30">
         <v>0.28899999999999998</v>
       </c>
-      <c r="M37" s="6"/>
+      <c r="M37" s="30">
+        <v>0.191</v>
+      </c>
       <c r="N37" s="6">
         <v>15.36</v>
       </c>
@@ -2183,7 +2238,7 @@
       </c>
       <c r="S37" s="6"/>
     </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>42617</v>
       </c>
@@ -2203,10 +2258,12 @@
       <c r="K38" s="6">
         <v>24</v>
       </c>
-      <c r="L38" s="6">
+      <c r="L38" s="30">
         <v>0.17599999999999999</v>
       </c>
-      <c r="M38" s="6"/>
+      <c r="M38" s="30">
+        <v>0.184</v>
+      </c>
       <c r="N38" s="6">
         <v>10.88</v>
       </c>
@@ -2224,7 +2281,7 @@
       </c>
       <c r="S38" s="6"/>
     </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>42617</v>
       </c>
@@ -2244,10 +2301,12 @@
       <c r="K39" s="6">
         <v>29.5</v>
       </c>
-      <c r="L39" s="6">
+      <c r="L39" s="30">
         <v>0.46500000000000002</v>
       </c>
-      <c r="M39" s="6"/>
+      <c r="M39" s="30">
+        <v>0.23</v>
+      </c>
       <c r="N39" s="6">
         <v>13.29</v>
       </c>
@@ -2265,7 +2324,7 @@
       </c>
       <c r="S39" s="6"/>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42617</v>
       </c>
@@ -2278,10 +2337,12 @@
       <c r="K40" s="3">
         <v>22</v>
       </c>
-      <c r="L40" s="7">
+      <c r="L40" s="30">
         <v>0.13900000000000001</v>
       </c>
-      <c r="M40" s="7"/>
+      <c r="M40" s="30">
+        <v>0.192</v>
+      </c>
       <c r="N40" s="7">
         <v>-4.01</v>
       </c>
@@ -2299,7 +2360,7 @@
       </c>
       <c r="S40" s="7"/>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42617</v>
       </c>
@@ -2312,10 +2373,12 @@
       <c r="K41" s="3">
         <v>24</v>
       </c>
-      <c r="L41" s="7">
+      <c r="L41" s="30">
         <v>0.48399999999999999</v>
       </c>
-      <c r="M41" s="7"/>
+      <c r="M41" s="30">
+        <v>0.26300000000000001</v>
+      </c>
       <c r="N41" s="7">
         <v>-4.05</v>
       </c>
@@ -2333,7 +2396,7 @@
       </c>
       <c r="S41" s="7"/>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42617</v>
       </c>
@@ -2346,10 +2409,12 @@
       <c r="K42" s="3">
         <v>5</v>
       </c>
-      <c r="L42" s="7">
+      <c r="L42" s="30">
         <v>0.84399999999999997</v>
       </c>
-      <c r="M42" s="7"/>
+      <c r="M42" s="30">
+        <v>-1.4E-2</v>
+      </c>
       <c r="N42" s="7">
         <v>-3.35</v>
       </c>
@@ -2369,7 +2434,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42617</v>
       </c>
@@ -2379,12 +2444,14 @@
       <c r="D43" s="7">
         <v>4</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="30">
         <f>1576.46+1778.84-195.36-194.86</f>
         <v>2965.08</v>
       </c>
       <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
+      <c r="M43" s="30">
+        <v>0</v>
+      </c>
       <c r="N43" s="7">
         <v>-3.74</v>
       </c>
@@ -2401,8 +2468,11 @@
         <v>0.61</v>
       </c>
       <c r="S43" s="7"/>
-    </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42617</v>
       </c>
@@ -2412,10 +2482,12 @@
       <c r="D44" s="7">
         <v>4</v>
       </c>
-      <c r="L44" s="7">
+      <c r="L44" s="30">
         <v>1.3460000000000001</v>
       </c>
-      <c r="M44" s="7"/>
+      <c r="M44" s="30">
+        <v>-3.9E-2</v>
+      </c>
       <c r="N44" s="7">
         <v>-4.62</v>
       </c>
@@ -2433,7 +2505,7 @@
       </c>
       <c r="S44" s="7"/>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42617</v>
       </c>
@@ -2443,10 +2515,12 @@
       <c r="D45" s="7">
         <v>4</v>
       </c>
-      <c r="L45" s="7">
+      <c r="L45" s="30">
         <v>0.59799999999999998</v>
       </c>
-      <c r="M45" s="7"/>
+      <c r="M45" s="30">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="N45" s="12">
         <v>18.04</v>
       </c>
@@ -2464,7 +2538,7 @@
       </c>
       <c r="S45" s="7"/>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42671</v>
       </c>
@@ -2474,10 +2548,10 @@
       <c r="D46" s="7">
         <v>5</v>
       </c>
-      <c r="L46" s="7">
+      <c r="L46" s="30">
         <v>-4.2999999999999997E-2</v>
       </c>
-      <c r="M46" s="7">
+      <c r="M46" s="30">
         <v>0.157</v>
       </c>
       <c r="N46" s="7"/>
@@ -2492,7 +2566,7 @@
         <v>-5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>42671</v>
       </c>
@@ -2502,10 +2576,10 @@
       <c r="D47" s="7">
         <v>5</v>
       </c>
-      <c r="L47" s="7">
+      <c r="L47" s="30">
         <v>-4.2999999999999997E-2</v>
       </c>
-      <c r="M47" s="7">
+      <c r="M47" s="30">
         <v>0.157</v>
       </c>
       <c r="N47" s="7"/>
@@ -2517,7 +2591,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>42671</v>
       </c>
@@ -2528,7 +2602,10 @@
       <c r="D48" s="6">
         <v>5</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="33">
+        <f>SUM(U48:X48)</f>
+        <v>82.922942715905791</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6">
@@ -2543,10 +2620,10 @@
       <c r="K48" s="6">
         <v>25</v>
       </c>
-      <c r="L48" s="6">
+      <c r="L48" s="30">
         <v>0.374</v>
       </c>
-      <c r="M48" s="6">
+      <c r="M48" s="30">
         <v>0.40300000000000002</v>
       </c>
       <c r="N48" s="6"/>
@@ -2557,8 +2634,24 @@
       <c r="S48" s="6">
         <v>0.17799999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U48" s="32">
+        <f>(H48-0.6078)/1.3756</f>
+        <v>26.092032567606864</v>
+      </c>
+      <c r="V48" s="32">
+        <f t="shared" ref="V48:V50" si="0">(I48-0.6078)/1.3756</f>
+        <v>22.093777260831637</v>
+      </c>
+      <c r="W48" s="32">
+        <f t="shared" ref="W48:W49" si="1">(J48-0.6078)/1.3756</f>
+        <v>17.005088688572261</v>
+      </c>
+      <c r="X48" s="32">
+        <f t="shared" ref="X48:X50" si="2">(K48-0.6078)/1.3756</f>
+        <v>17.732044198895029</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>42671</v>
       </c>
@@ -2569,7 +2662,10 @@
       <c r="D49" s="6">
         <v>5</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="33">
+        <f t="shared" ref="E49:E50" si="3">SUM(U49:X49)</f>
+        <v>74.562954347193966</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6">
@@ -2584,10 +2680,10 @@
       <c r="K49" s="6">
         <v>24</v>
       </c>
-      <c r="L49" s="6">
+      <c r="L49" s="30">
         <v>0.42399999999999999</v>
       </c>
-      <c r="M49" s="6">
+      <c r="M49" s="30">
         <v>0.67600000000000005</v>
       </c>
       <c r="N49" s="6"/>
@@ -2598,8 +2694,24 @@
       <c r="S49" s="6">
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U49" s="32">
+        <f>(H49-0.6078)/1.3756</f>
+        <v>14.097266647281186</v>
+      </c>
+      <c r="V49" s="32">
+        <f t="shared" si="0"/>
+        <v>30.090287874382092</v>
+      </c>
+      <c r="W49" s="32">
+        <f t="shared" si="1"/>
+        <v>13.370311136958419</v>
+      </c>
+      <c r="X49" s="32">
+        <f t="shared" si="2"/>
+        <v>17.005088688572261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>42671</v>
       </c>
@@ -2610,7 +2722,10 @@
       <c r="D50" s="6">
         <v>5</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="33">
+        <f t="shared" si="3"/>
+        <v>82.559464960744407</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6">
@@ -2625,10 +2740,10 @@
       <c r="K50" s="6">
         <v>18</v>
       </c>
-      <c r="L50" s="6">
+      <c r="L50" s="30">
         <v>0.50800000000000001</v>
       </c>
-      <c r="M50" s="6">
+      <c r="M50" s="30">
         <v>1.097</v>
       </c>
       <c r="N50" s="6"/>
@@ -2639,8 +2754,24 @@
       <c r="S50" s="6">
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U50" s="32">
+        <f t="shared" ref="U50" si="4">(H50-0.6078)/1.3756</f>
+        <v>18.458999709217796</v>
+      </c>
+      <c r="V50" s="32">
+        <f t="shared" si="0"/>
+        <v>25.728554812445481</v>
+      </c>
+      <c r="W50" s="32">
+        <f>(J50-0.6078)/1.3756</f>
+        <v>25.728554812445481</v>
+      </c>
+      <c r="X50" s="32">
+        <f t="shared" si="2"/>
+        <v>12.64335562663565</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>42671</v>
       </c>
@@ -2650,13 +2781,17 @@
       <c r="D51" s="7">
         <v>5</v>
       </c>
+      <c r="E51" s="33">
+        <f>(H51-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
       <c r="H51" s="3">
         <v>14</v>
       </c>
-      <c r="L51" s="7">
+      <c r="L51" s="30">
         <v>0.39400000000000002</v>
       </c>
-      <c r="M51" s="7">
+      <c r="M51" s="30">
         <v>2.7080000000000002</v>
       </c>
       <c r="N51" s="7"/>
@@ -2671,7 +2806,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>42671</v>
       </c>
@@ -2681,13 +2816,17 @@
       <c r="D52" s="7">
         <v>5</v>
       </c>
+      <c r="E52" s="33">
+        <f t="shared" ref="E51:E53" si="5">(H52-0.6078)/1.3756</f>
+        <v>28.636376853736554</v>
+      </c>
       <c r="H52" s="3">
         <v>40</v>
       </c>
-      <c r="L52" s="7">
+      <c r="L52" s="30">
         <v>0.13400000000000001</v>
       </c>
-      <c r="M52" s="7">
+      <c r="M52" s="30">
         <v>6.3259999999999996</v>
       </c>
       <c r="N52" s="7"/>
@@ -2702,7 +2841,7 @@
         <v>-5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>42671</v>
       </c>
@@ -2712,13 +2851,17 @@
       <c r="D53" s="7">
         <v>5</v>
       </c>
+      <c r="E53" s="33">
+        <f t="shared" si="5"/>
+        <v>17.005088688572261</v>
+      </c>
       <c r="H53" s="3">
         <v>24</v>
       </c>
-      <c r="L53" s="7">
+      <c r="L53" s="30">
         <v>0.438</v>
       </c>
-      <c r="M53" s="7">
+      <c r="M53" s="30">
         <v>6.1669999999999998</v>
       </c>
       <c r="N53" s="7"/>
@@ -2730,7 +2873,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>42671</v>
       </c>
@@ -2740,10 +2883,10 @@
       <c r="D54" s="7">
         <v>5</v>
       </c>
-      <c r="L54" s="7">
+      <c r="L54" s="30">
         <v>0.20899999999999999</v>
       </c>
-      <c r="M54" s="7">
+      <c r="M54" s="30">
         <v>2.35</v>
       </c>
       <c r="N54" s="7"/>
@@ -2755,7 +2898,7 @@
         <v>-0.308</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42671</v>
       </c>
@@ -2774,7 +2917,7 @@
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42671</v>
       </c>
@@ -2793,7 +2936,7 @@
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>42723</v>
       </c>
@@ -2803,10 +2946,10 @@
       <c r="D57" s="7">
         <v>6</v>
       </c>
-      <c r="L57" s="7">
+      <c r="L57" s="30">
         <v>2.4E-2</v>
       </c>
-      <c r="M57" s="7">
+      <c r="M57" s="30">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N57" s="7"/>
@@ -2816,7 +2959,7 @@
       <c r="R57" s="7"/>
       <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42723</v>
       </c>
@@ -2826,10 +2969,10 @@
       <c r="D58" s="7">
         <v>6</v>
       </c>
-      <c r="L58" s="7">
+      <c r="L58" s="30">
         <v>2.4E-2</v>
       </c>
-      <c r="M58" s="7">
+      <c r="M58" s="30">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N58" s="7"/>
@@ -2839,7 +2982,7 @@
       <c r="R58" s="7"/>
       <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>42723</v>
       </c>
@@ -2850,7 +2993,10 @@
       <c r="D59" s="6">
         <v>6</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="33">
+        <f>SUM(U59:X59)</f>
+        <v>46.211689444605994</v>
+      </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6">
@@ -2865,10 +3011,10 @@
       <c r="K59" s="6">
         <v>18</v>
       </c>
-      <c r="L59" s="6">
+      <c r="L59" s="30">
         <v>0.498</v>
       </c>
-      <c r="M59" s="6">
+      <c r="M59" s="30">
         <v>0.29699999999999999</v>
       </c>
       <c r="N59" s="6"/>
@@ -2877,8 +3023,24 @@
       <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
       <c r="S59" s="6"/>
-    </row>
-    <row r="60" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U59" s="32">
+        <f>(H59-0.6078)/1.3756</f>
+        <v>11.916400116312882</v>
+      </c>
+      <c r="V59" s="32">
+        <f t="shared" ref="V59:V61" si="6">(I59-0.6078)/1.3756</f>
+        <v>10.462489095667346</v>
+      </c>
+      <c r="W59" s="32">
+        <f t="shared" ref="W59:W60" si="7">(J59-0.6078)/1.3756</f>
+        <v>11.189444605990115</v>
+      </c>
+      <c r="X59" s="32">
+        <f t="shared" ref="X59:X61" si="8">(K59-0.6078)/1.3756</f>
+        <v>12.64335562663565</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>42723</v>
       </c>
@@ -2889,7 +3051,10 @@
       <c r="D60" s="6">
         <v>6</v>
       </c>
-      <c r="E60" s="6"/>
+      <c r="E60" s="33">
+        <f t="shared" ref="E60:E61" si="9">SUM(U60:X60)</f>
+        <v>32.3995347484734</v>
+      </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6">
@@ -2904,10 +3069,10 @@
       <c r="K60" s="6">
         <v>10</v>
       </c>
-      <c r="L60" s="6">
+      <c r="L60" s="30">
         <v>0.13300000000000001</v>
       </c>
-      <c r="M60" s="6">
+      <c r="M60" s="30">
         <v>0.107</v>
       </c>
       <c r="N60" s="6"/>
@@ -2916,8 +3081,24 @@
       <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
-    </row>
-    <row r="61" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U60" s="32">
+        <f>(H60-0.6078)/1.3756</f>
+        <v>6.1007560337307369</v>
+      </c>
+      <c r="V60" s="32">
+        <f t="shared" si="6"/>
+        <v>14.097266647281186</v>
+      </c>
+      <c r="W60" s="32">
+        <f t="shared" si="7"/>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="X60" s="32">
+        <f t="shared" si="8"/>
+        <v>6.8277115440535052</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>42723</v>
       </c>
@@ -2928,7 +3109,10 @@
       <c r="D61" s="6">
         <v>6</v>
       </c>
-      <c r="E61" s="6"/>
+      <c r="E61" s="33">
+        <f t="shared" si="9"/>
+        <v>37.488223320732779</v>
+      </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6">
@@ -2943,10 +3127,10 @@
       <c r="K61" s="6">
         <v>9</v>
       </c>
-      <c r="L61" s="6">
+      <c r="L61" s="30">
         <v>0.51500000000000001</v>
       </c>
-      <c r="M61" s="6">
+      <c r="M61" s="30">
         <v>0.19500000000000001</v>
       </c>
       <c r="N61" s="6"/>
@@ -2955,8 +3139,24 @@
       <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
-    </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U61" s="32">
+        <f t="shared" ref="U61" si="10">(H61-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
+      <c r="V61" s="32">
+        <f t="shared" si="6"/>
+        <v>9.7355335853445784</v>
+      </c>
+      <c r="W61" s="32">
+        <f>(J61-0.6078)/1.3756</f>
+        <v>11.916400116312882</v>
+      </c>
+      <c r="X61" s="32">
+        <f t="shared" si="8"/>
+        <v>6.1007560337307369</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42723</v>
       </c>
@@ -2966,13 +3166,13 @@
       <c r="D62" s="7">
         <v>6</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="30">
         <v>4</v>
       </c>
-      <c r="L62" s="7">
+      <c r="L62" s="30">
         <v>0.83899999999999997</v>
       </c>
-      <c r="M62" s="7">
+      <c r="M62" s="30">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="N62" s="7"/>
@@ -2982,7 +3182,7 @@
       <c r="R62" s="7"/>
       <c r="S62" s="7"/>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42723</v>
       </c>
@@ -2992,13 +3192,19 @@
       <c r="D63" s="7">
         <v>6</v>
       </c>
-      <c r="H63" s="3">
+      <c r="E63" s="35">
+        <f>(H63-0.6078)/1.3756</f>
+        <v>26.455510322768248</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="36">
         <v>37</v>
       </c>
-      <c r="L63" s="7">
+      <c r="L63" s="30">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M63" s="7">
+      <c r="M63" s="30">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="N63" s="7"/>
@@ -3008,7 +3214,7 @@
       <c r="R63" s="7"/>
       <c r="S63" s="7"/>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42723</v>
       </c>
@@ -3018,13 +3224,13 @@
       <c r="D64" s="7">
         <v>6</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="30">
         <v>8</v>
       </c>
-      <c r="L64" s="7">
+      <c r="L64" s="30">
         <v>0.182</v>
       </c>
-      <c r="M64" s="7">
+      <c r="M64" s="30">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="N64" s="7"/>
@@ -3034,7 +3240,7 @@
       <c r="R64" s="7"/>
       <c r="S64" s="7"/>
     </row>
-    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42723</v>
       </c>
@@ -3048,10 +3254,10 @@
         <f>987+2922.54-193.67-194.18</f>
         <v>3521.69</v>
       </c>
-      <c r="L65" s="7">
+      <c r="L65" s="30">
         <v>0.253</v>
       </c>
-      <c r="M65" s="7">
+      <c r="M65" s="30">
         <v>1.161</v>
       </c>
       <c r="N65" s="7"/>
@@ -3063,7 +3269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42723</v>
       </c>
@@ -3073,10 +3279,10 @@
       <c r="D66" s="7">
         <v>6</v>
       </c>
-      <c r="L66" s="7">
+      <c r="L66" s="30">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="M66" s="7">
+      <c r="M66" s="30">
         <v>0.77200000000000002</v>
       </c>
       <c r="N66" s="7"/>
@@ -3086,7 +3292,7 @@
       <c r="R66" s="7"/>
       <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42723</v>
       </c>
@@ -3105,7 +3311,7 @@
       <c r="R67" s="7"/>
       <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42800</v>
       </c>
@@ -3115,11 +3321,11 @@
       <c r="D68" s="7">
         <v>7</v>
       </c>
-      <c r="L68" s="7">
+      <c r="L68" s="30">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="M68" s="7">
-        <v>4.4999999999999997E-3</v>
+      <c r="M68" s="30">
+        <v>-1.35E-2</v>
       </c>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -3127,8 +3333,12 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="7"/>
       <c r="S68" s="7"/>
-    </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y68">
+        <f>(-0.031+0.004)/2</f>
+        <v>-1.35E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42800</v>
       </c>
@@ -3138,11 +3348,11 @@
       <c r="D69" s="7">
         <v>7</v>
       </c>
-      <c r="L69" s="7">
+      <c r="L69" s="30">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="M69" s="7">
-        <v>4.4999999999999997E-3</v>
+      <c r="M69" s="30">
+        <v>-1.35E-2</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -3151,7 +3361,7 @@
       <c r="R69" s="7"/>
       <c r="S69" s="7"/>
     </row>
-    <row r="70" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>42800</v>
       </c>
@@ -3162,7 +3372,10 @@
       <c r="D70" s="7">
         <v>7</v>
       </c>
-      <c r="E70" s="6"/>
+      <c r="E70" s="33">
+        <f>SUM(U70:X70)</f>
+        <v>41.123000872346616</v>
+      </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6">
@@ -3177,10 +3390,10 @@
       <c r="K70" s="6">
         <v>14</v>
       </c>
-      <c r="L70" s="6">
+      <c r="L70" s="30">
         <v>1.1579999999999999</v>
       </c>
-      <c r="M70" s="6">
+      <c r="M70" s="30">
         <v>6.27</v>
       </c>
       <c r="N70" s="6"/>
@@ -3189,8 +3402,27 @@
       <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
       <c r="S70" s="6"/>
-    </row>
-    <row r="71" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U70" s="32">
+        <f>(H70-0.6078)/1.3756</f>
+        <v>12.64335562663565</v>
+      </c>
+      <c r="V70" s="32">
+        <f t="shared" ref="V70:V72" si="11">(I70-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
+      <c r="W70" s="32">
+        <f t="shared" ref="W70:W71" si="12">(J70-0.6078)/1.3756</f>
+        <v>9.0085780750218092</v>
+      </c>
+      <c r="X70" s="32">
+        <f t="shared" ref="X70:X72" si="13">(K70-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>42800</v>
       </c>
@@ -3201,7 +3433,10 @@
       <c r="D71" s="7">
         <v>7</v>
       </c>
-      <c r="E71" s="6"/>
+      <c r="E71" s="33">
+        <f t="shared" ref="E71:E72" si="14">SUM(U71:X71)</f>
+        <v>41.123000872346616</v>
+      </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6">
@@ -3216,10 +3451,10 @@
       <c r="K71" s="6">
         <v>11</v>
       </c>
-      <c r="L71" s="6">
+      <c r="L71" s="30">
         <v>1.105</v>
       </c>
-      <c r="M71" s="6">
+      <c r="M71" s="30">
         <v>7.02</v>
       </c>
       <c r="N71" s="6"/>
@@ -3228,8 +3463,24 @@
       <c r="Q71" s="6"/>
       <c r="R71" s="6"/>
       <c r="S71" s="6"/>
-    </row>
-    <row r="72" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U71" s="32">
+        <f>(H71-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
+      <c r="V71" s="32">
+        <f t="shared" si="11"/>
+        <v>9.0085780750218092</v>
+      </c>
+      <c r="W71" s="32">
+        <f t="shared" si="12"/>
+        <v>14.824222157603955</v>
+      </c>
+      <c r="X71" s="32">
+        <f t="shared" si="13"/>
+        <v>7.5546670543762735</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>42800</v>
       </c>
@@ -3240,7 +3491,10 @@
       <c r="D72" s="7">
         <v>7</v>
       </c>
-      <c r="E72" s="6"/>
+      <c r="E72" s="33">
+        <f t="shared" si="14"/>
+        <v>46.211689444605994</v>
+      </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
       <c r="H72" s="6">
@@ -3255,10 +3509,10 @@
       <c r="K72" s="6">
         <v>19</v>
       </c>
-      <c r="L72" s="6">
+      <c r="L72" s="30">
         <v>1.2809999999999999</v>
       </c>
-      <c r="M72" s="6">
+      <c r="M72" s="30">
         <v>6.84</v>
       </c>
       <c r="N72" s="6"/>
@@ -3267,8 +3521,24 @@
       <c r="Q72" s="6"/>
       <c r="R72" s="6"/>
       <c r="S72" s="6"/>
-    </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U72" s="32">
+        <f t="shared" ref="U72" si="15">(H72-0.6078)/1.3756</f>
+        <v>9.7355335853445784</v>
+      </c>
+      <c r="V72" s="32">
+        <f t="shared" si="11"/>
+        <v>12.64335562663565</v>
+      </c>
+      <c r="W72" s="32">
+        <f>(J72-0.6078)/1.3756</f>
+        <v>10.462489095667346</v>
+      </c>
+      <c r="X72" s="32">
+        <f t="shared" si="13"/>
+        <v>13.370311136958419</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>42800</v>
       </c>
@@ -3278,13 +3548,17 @@
       <c r="D73" s="7">
         <v>7</v>
       </c>
+      <c r="E73" s="33">
+        <f t="shared" ref="E73:E75" si="16">(H73-0.6078)/1.3756</f>
+        <v>27.182465833091019</v>
+      </c>
       <c r="H73" s="3">
         <v>38</v>
       </c>
-      <c r="L73" s="7">
+      <c r="L73" s="30">
         <v>0.11899999999999999</v>
       </c>
-      <c r="M73" s="7">
+      <c r="M73" s="30">
         <v>11.94</v>
       </c>
       <c r="N73" s="7"/>
@@ -3294,7 +3568,7 @@
       <c r="R73" s="7"/>
       <c r="S73" s="7"/>
     </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>42800</v>
       </c>
@@ -3304,13 +3578,17 @@
       <c r="D74" s="7">
         <v>7</v>
       </c>
+      <c r="E74" s="33">
+        <f t="shared" si="16"/>
+        <v>16.27813317824949</v>
+      </c>
       <c r="H74" s="3">
         <v>23</v>
       </c>
-      <c r="L74" s="7">
+      <c r="L74" s="30">
         <v>0.11899999999999999</v>
       </c>
-      <c r="M74" s="7">
+      <c r="M74" s="30">
         <v>23.13</v>
       </c>
       <c r="N74" s="7"/>
@@ -3320,7 +3598,7 @@
       <c r="R74" s="7"/>
       <c r="S74" s="7"/>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>42800</v>
       </c>
@@ -3330,13 +3608,17 @@
       <c r="D75" s="7">
         <v>7</v>
       </c>
+      <c r="E75" s="33">
+        <f t="shared" si="16"/>
+        <v>9.7355335853445784</v>
+      </c>
       <c r="H75" s="3">
         <v>14</v>
       </c>
-      <c r="L75" s="7">
+      <c r="L75" s="30">
         <v>0.129</v>
       </c>
-      <c r="M75" s="7">
+      <c r="M75" s="30">
         <v>2.0499999999999998</v>
       </c>
       <c r="N75" s="7"/>
@@ -3346,7 +3628,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="7"/>
     </row>
-    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>42800</v>
       </c>
@@ -3356,11 +3638,11 @@
       <c r="D76" s="7">
         <v>7</v>
       </c>
-      <c r="L76" s="7">
+      <c r="L76" s="30">
         <v>0.13500000000000001</v>
       </c>
-      <c r="M76" s="7">
-        <v>0.84</v>
+      <c r="M76" s="30">
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3369,7 +3651,7 @@
       <c r="R76" s="7"/>
       <c r="S76" s="7"/>
     </row>
-    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>42800</v>
       </c>
@@ -3388,7 +3670,7 @@
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>42800</v>
       </c>
@@ -3407,7 +3689,7 @@
       <c r="R78" s="7"/>
       <c r="S78" s="7"/>
     </row>
-    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>42671</v>
       </c>
@@ -3430,7 +3712,7 @@
       <c r="R79" s="7"/>
       <c r="S79" s="7"/>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>42671</v>
       </c>
@@ -3680,9 +3962,9 @@
       <c r="R89" s="7"/>
       <c r="S89" s="7"/>
     </row>
-    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>42800</v>
+        <v>42807</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>5</v>
@@ -3705,9 +3987,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>42800</v>
+        <v>42807</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>5</v>
@@ -3728,7 +4010,7 @@
       <c r="R91" s="7"/>
       <c r="S91" s="7"/>
     </row>
-    <row r="92" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>42807</v>
       </c>
@@ -3736,8 +4018,10 @@
         <v>6</v>
       </c>
       <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6">
+      <c r="D92" s="6">
+        <v>9</v>
+      </c>
+      <c r="E92" s="30">
         <v>7.5</v>
       </c>
       <c r="F92" s="6"/>
@@ -3754,10 +4038,10 @@
       <c r="K92" s="6">
         <v>3</v>
       </c>
-      <c r="L92" s="6">
+      <c r="L92" s="30">
         <v>0.16700000000000001</v>
       </c>
-      <c r="M92" s="6">
+      <c r="M92" s="30">
         <v>0.26700000000000002</v>
       </c>
       <c r="N92" s="6"/>
@@ -3769,7 +4053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>42807</v>
       </c>
@@ -3777,8 +4061,10 @@
         <v>7</v>
       </c>
       <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6">
+      <c r="D93" s="6">
+        <v>9</v>
+      </c>
+      <c r="E93" s="30">
         <v>7</v>
       </c>
       <c r="F93" s="6"/>
@@ -3795,10 +4081,10 @@
       <c r="K93" s="6">
         <v>2</v>
       </c>
-      <c r="L93" s="6">
+      <c r="L93" s="30">
         <v>0.17599999999999999</v>
       </c>
-      <c r="M93" s="6">
+      <c r="M93" s="30">
         <v>0.248</v>
       </c>
       <c r="N93" s="6"/>
@@ -3810,7 +4096,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:19" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>42807</v>
       </c>
@@ -3818,8 +4104,10 @@
         <v>8</v>
       </c>
       <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6">
+      <c r="D94" s="6">
+        <v>9</v>
+      </c>
+      <c r="E94" s="30">
         <v>7.8</v>
       </c>
       <c r="F94" s="6"/>
@@ -3836,10 +4124,10 @@
       <c r="K94" s="6">
         <v>4</v>
       </c>
-      <c r="L94" s="6">
+      <c r="L94" s="30">
         <v>0.183</v>
       </c>
-      <c r="M94" s="6">
+      <c r="M94" s="30">
         <v>0.28999999999999998</v>
       </c>
       <c r="N94" s="6"/>
@@ -3851,23 +4139,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>42807</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E95" s="7">
+      <c r="D95" s="7">
+        <v>9</v>
+      </c>
+      <c r="E95" s="30">
         <v>5</v>
       </c>
       <c r="H95" s="3">
         <v>9</v>
       </c>
-      <c r="L95" s="7">
+      <c r="L95" s="30">
         <v>0.13200000000000001</v>
       </c>
-      <c r="M95" s="7">
+      <c r="M95" s="30">
         <v>0.24299999999999999</v>
       </c>
       <c r="N95" s="7"/>
@@ -3877,23 +4168,26 @@
       <c r="R95" s="7"/>
       <c r="S95" s="7"/>
     </row>
-    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>42807</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E96" s="7">
+      <c r="D96" s="7">
+        <v>9</v>
+      </c>
+      <c r="E96" s="30">
         <v>7</v>
       </c>
       <c r="H96" s="3">
         <v>11</v>
       </c>
-      <c r="L96" s="7">
+      <c r="L96" s="30">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="M96" s="7">
+      <c r="M96" s="30">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="N96" s="7"/>
@@ -3903,23 +4197,26 @@
       <c r="R96" s="7"/>
       <c r="S96" s="7"/>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>42807</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E97" s="7">
+      <c r="D97" s="7">
+        <v>9</v>
+      </c>
+      <c r="E97" s="30">
         <v>5</v>
       </c>
       <c r="H97" s="3">
         <v>2</v>
       </c>
-      <c r="L97" s="7">
+      <c r="L97" s="30">
         <v>0.14099999999999999</v>
       </c>
-      <c r="M97" s="7">
+      <c r="M97" s="30">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="N97" s="7"/>
@@ -3929,20 +4226,23 @@
       <c r="R97" s="7"/>
       <c r="S97" s="7"/>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>42807</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="7">
+      <c r="D98" s="7">
+        <v>9</v>
+      </c>
+      <c r="E98" s="30">
         <v>1.45</v>
       </c>
-      <c r="L98" s="7">
+      <c r="L98" s="30">
         <v>0.20599999999999999</v>
       </c>
-      <c r="M98" s="7">
+      <c r="M98" s="30">
         <v>0.63400000000000001</v>
       </c>
       <c r="N98" s="7"/>
@@ -3952,20 +4252,23 @@
       <c r="R98" s="7"/>
       <c r="S98" s="7"/>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>42807</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="D99" s="7">
+        <v>9</v>
+      </c>
       <c r="E99" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L99" s="7">
+      <c r="L99" s="30">
         <v>0.13</v>
       </c>
-      <c r="M99" s="7">
+      <c r="M99" s="30">
         <v>0.22600000000000001</v>
       </c>
       <c r="N99" s="7"/>
@@ -3975,17 +4278,20 @@
       <c r="R99" s="7"/>
       <c r="S99" s="7"/>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>42807</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L100" s="7">
+      <c r="D100" s="7">
+        <v>9</v>
+      </c>
+      <c r="L100" s="30">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="M100" s="7">
+      <c r="M100" s="30">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="N100" s="7"/>
@@ -3995,15 +4301,22 @@
       <c r="R100" s="7"/>
       <c r="S100" s="7"/>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>42831</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L101" s="7"/>
-      <c r="M101" s="7"/>
+      <c r="D101" s="7">
+        <v>10</v>
+      </c>
+      <c r="L101" s="30">
+        <v>-6.8000000000000005E-2</v>
+      </c>
+      <c r="M101" s="30">
+        <v>-6.3E-2</v>
+      </c>
       <c r="N101" s="7"/>
       <c r="O101" s="7"/>
       <c r="P101" s="7"/>
@@ -4011,25 +4324,32 @@
       <c r="R101" s="7"/>
       <c r="S101" s="7"/>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>42831</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L102" s="7"/>
-      <c r="M102" s="7">
-        <v>1</v>
+      <c r="D102" s="7">
+        <v>10</v>
+      </c>
+      <c r="L102" s="30">
+        <v>-6.8000000000000005E-2</v>
+      </c>
+      <c r="M102" s="30">
+        <v>-6.3E-2</v>
       </c>
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
       <c r="P102" s="7"/>
       <c r="Q102" s="7"/>
       <c r="R102" s="7"/>
-      <c r="S102" s="7"/>
-    </row>
-    <row r="103" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S102" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>42831</v>
       </c>
@@ -4037,8 +4357,13 @@
         <v>6</v>
       </c>
       <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
+      <c r="D103" s="6">
+        <v>10</v>
+      </c>
+      <c r="E103" s="33">
+        <f>SUM(U103:X103)</f>
+        <v>24.403024134922948</v>
+      </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
       <c r="H103" s="6">
@@ -4053,18 +4378,38 @@
       <c r="K103" s="6">
         <v>8</v>
       </c>
-      <c r="L103" s="6"/>
-      <c r="M103" s="6">
-        <v>2</v>
+      <c r="L103" s="30">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="M103" s="30">
+        <v>0.152</v>
       </c>
       <c r="N103" s="6"/>
       <c r="O103" s="6"/>
       <c r="P103" s="6"/>
       <c r="Q103" s="6"/>
       <c r="R103" s="6"/>
-      <c r="S103" s="6"/>
-    </row>
-    <row r="104" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S103" s="6">
+        <v>2</v>
+      </c>
+      <c r="U103" s="32">
+        <f>(H103-0.6078)/1.3756</f>
+        <v>7.5546670543762735</v>
+      </c>
+      <c r="V103" s="32">
+        <f t="shared" ref="V103:X103" si="17">(I103-0.6078)/1.3756</f>
+        <v>6.1007560337307369</v>
+      </c>
+      <c r="W103" s="32">
+        <f t="shared" si="17"/>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="X103" s="32">
+        <f t="shared" si="17"/>
+        <v>5.3738005234079678</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>42831</v>
       </c>
@@ -4072,8 +4417,13 @@
         <v>7</v>
       </c>
       <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
+      <c r="D104" s="6">
+        <v>10</v>
+      </c>
+      <c r="E104" s="33">
+        <f t="shared" ref="E104:E105" si="18">SUM(U104:X104)</f>
+        <v>22.222157603954638</v>
+      </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
       <c r="H104" s="6">
@@ -4088,18 +4438,38 @@
       <c r="K104" s="6">
         <v>6</v>
       </c>
-      <c r="L104" s="6"/>
-      <c r="M104" s="6">
-        <v>3</v>
+      <c r="L104" s="30">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="M104" s="30">
+        <v>0.17899999999999999</v>
       </c>
       <c r="N104" s="6"/>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
       <c r="Q104" s="6"/>
       <c r="R104" s="6"/>
-      <c r="S104" s="6"/>
-    </row>
-    <row r="105" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S104" s="6">
+        <v>3</v>
+      </c>
+      <c r="U104" s="32">
+        <f>(H104-0.6078)/1.3756</f>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="V104" s="32">
+        <f t="shared" ref="V104:V105" si="19">(I104-0.6078)/1.3756</f>
+        <v>3.9198895027624312</v>
+      </c>
+      <c r="W104" s="32">
+        <f t="shared" ref="W104:W105" si="20">(J104-0.6078)/1.3756</f>
+        <v>9.0085780750218092</v>
+      </c>
+      <c r="X104" s="32">
+        <f t="shared" ref="X104:X105" si="21">(K104-0.6078)/1.3756</f>
+        <v>3.9198895027624312</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>42831</v>
       </c>
@@ -4107,8 +4477,13 @@
         <v>8</v>
       </c>
       <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
+      <c r="D105" s="6">
+        <v>10</v>
+      </c>
+      <c r="E105" s="33">
+        <f t="shared" si="18"/>
+        <v>25.129979645245715</v>
+      </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
       <c r="H105" s="6">
@@ -4123,135 +4498,209 @@
       <c r="K105" s="6">
         <v>11</v>
       </c>
-      <c r="L105" s="6"/>
-      <c r="M105" s="6">
-        <v>4</v>
+      <c r="L105" s="30">
+        <v>0.249</v>
+      </c>
+      <c r="M105" s="30">
+        <v>0.251</v>
       </c>
       <c r="N105" s="6"/>
       <c r="O105" s="6"/>
       <c r="P105" s="6"/>
       <c r="Q105" s="6"/>
       <c r="R105" s="6"/>
-      <c r="S105" s="6"/>
-    </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S105" s="6">
+        <v>4</v>
+      </c>
+      <c r="U105" s="32">
+        <f t="shared" ref="U104:U105" si="22">(H105-0.6078)/1.3756</f>
+        <v>6.8277115440535052</v>
+      </c>
+      <c r="V105" s="32">
+        <f t="shared" si="19"/>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="W105" s="32">
+        <f>(J105-0.6078)/1.3756</f>
+        <v>5.3738005234079678</v>
+      </c>
+      <c r="X105" s="32">
+        <f t="shared" si="21"/>
+        <v>7.5546670543762735</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>42831</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="D106" s="7">
+        <v>10</v>
+      </c>
+      <c r="E106" s="33">
+        <f>(H106-0.6078)/1.3756</f>
+        <v>11.189444605990115</v>
+      </c>
       <c r="H106" s="3">
         <v>16</v>
       </c>
-      <c r="L106" s="7"/>
-      <c r="M106" s="7">
-        <v>5</v>
+      <c r="L106" s="30">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="M106" s="30">
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
       <c r="P106" s="7"/>
       <c r="Q106" s="7"/>
       <c r="R106" s="7"/>
-      <c r="S106" s="7"/>
-    </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S106" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>42831</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="D107" s="7">
+        <v>10</v>
+      </c>
+      <c r="E107" s="33">
+        <f t="shared" ref="E107:E108" si="23">(H107-0.6078)/1.3756</f>
+        <v>22.093777260831637</v>
+      </c>
       <c r="H107" s="3">
         <v>31</v>
       </c>
-      <c r="L107" s="7"/>
-      <c r="M107" s="7">
-        <v>6</v>
+      <c r="L107" s="30">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="M107" s="30">
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
       <c r="P107" s="7"/>
       <c r="Q107" s="7"/>
       <c r="R107" s="7"/>
-      <c r="S107" s="7"/>
-    </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S107" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>42831</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="D108" s="7">
+        <v>10</v>
+      </c>
+      <c r="E108" s="33">
+        <f t="shared" si="23"/>
+        <v>4.6468450130851995</v>
+      </c>
       <c r="H108" s="3">
         <v>7</v>
       </c>
-      <c r="L108" s="7"/>
-      <c r="M108" s="7">
-        <v>7</v>
+      <c r="L108" s="30">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="M108" s="30">
+        <v>-1.2E-2</v>
       </c>
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
       <c r="P108" s="7"/>
       <c r="Q108" s="7"/>
       <c r="R108" s="7"/>
-      <c r="S108" s="7"/>
-    </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S108" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>42831</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L109" s="7"/>
-      <c r="M109" s="7">
+      <c r="D109" s="7">
         <v>10</v>
+      </c>
+      <c r="L109" s="30">
+        <v>0.215</v>
+      </c>
+      <c r="M109" s="30">
+        <v>0.69699999999999995</v>
       </c>
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
       <c r="P109" s="7"/>
       <c r="Q109" s="7"/>
       <c r="R109" s="7"/>
-      <c r="S109" s="7"/>
-    </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S109" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>42831</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L110" s="7"/>
-      <c r="M110" s="7">
-        <v>8</v>
+      <c r="D110" s="7">
+        <v>10</v>
+      </c>
+      <c r="L110" s="30">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="M110" s="30">
+        <v>0.24099999999999999</v>
       </c>
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
       <c r="P110" s="7"/>
       <c r="Q110" s="7"/>
       <c r="R110" s="7"/>
-      <c r="S110" s="7"/>
-    </row>
-    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S110" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>42831</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L111" s="7"/>
-      <c r="M111" s="7">
-        <v>9</v>
+      <c r="D111" s="7">
+        <v>10</v>
+      </c>
+      <c r="L111" s="30">
+        <v>2.4E-2</v>
+      </c>
+      <c r="M111" s="30">
+        <v>0.13300000000000001</v>
       </c>
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
       <c r="P111" s="7"/>
       <c r="Q111" s="7"/>
       <c r="R111" s="7"/>
-      <c r="S111" s="7"/>
-    </row>
-    <row r="112" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S111" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="24">
         <v>42592</v>
       </c>
@@ -4395,19 +4844,41 @@
       </c>
       <c r="S114" s="21"/>
     </row>
+    <row r="116" spans="1:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="38"/>
+      <c r="H116" s="38"/>
+      <c r="I116" s="38"/>
+      <c r="J116" s="38"/>
+      <c r="K116" s="38"/>
+      <c r="L116" s="38"/>
+      <c r="M116" s="38"/>
+      <c r="N116" s="38"/>
+      <c r="O116" s="38"/>
+      <c r="P116" s="38"/>
+      <c r="Q116" s="38"/>
+      <c r="R116" s="38"/>
+      <c r="S116" s="38"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D114">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="D1:D114"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
created a new .csv where I have all the key data to work on the summer spraying.
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
+++ b/15N_experiment/15N_fieldlab/15N_Ndep_db.xlsx
@@ -225,7 +225,7 @@
     <t>NOTA:(24/05/17): IO HO UN VOLUME ANCHE PER IL TF, CHE VA BENISSIMO, PERCHE' MI SERVIRA' PER CALCOLARE QUANTO N HO RACCOLTO: LA SUPERFICIE INTERCETTATA MI SERVIRA' SOLO PER CALCOLARE UN PARAMETRO PER SCALARIZZARE IL N RACCOLTO AL N TOTALE!!!</t>
   </si>
   <si>
-    <t>PER DOMANI 25/05: SPEDIRE I CAMPIONI, MAIL A CEH, POI PREPARARE IL DB "PULITO" SALVATO COME .csv</t>
+    <t>PER 26/05: SPEDIRE I CAMPIONI, MAIL A CEH, POI PREPARARE IL DB "PULITO" SALVATO COME .csv</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <dimension ref="A1:Y119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
@@ -2817,7 +2817,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="33">
-        <f t="shared" ref="E51:E53" si="5">(H52-0.6078)/1.3756</f>
+        <f t="shared" ref="E52:E53" si="5">(H52-0.6078)/1.3756</f>
         <v>28.636376853736554</v>
       </c>
       <c r="H52" s="3">
@@ -4461,7 +4461,7 @@
         <v>3.9198895027624312</v>
       </c>
       <c r="W104" s="32">
-        <f t="shared" ref="W104:W105" si="20">(J104-0.6078)/1.3756</f>
+        <f t="shared" ref="W104" si="20">(J104-0.6078)/1.3756</f>
         <v>9.0085780750218092</v>
       </c>
       <c r="X104" s="32">
@@ -4513,7 +4513,7 @@
         <v>4</v>
       </c>
       <c r="U105" s="32">
-        <f t="shared" ref="U104:U105" si="22">(H105-0.6078)/1.3756</f>
+        <f t="shared" ref="U105" si="22">(H105-0.6078)/1.3756</f>
         <v>6.8277115440535052</v>
       </c>
       <c r="V105" s="32">

</xml_diff>